<commit_message>
Resolved selenium e wd default
</commit_message>
<xml_diff>
--- a/sheets/lista.xlsx
+++ b/sheets/lista.xlsx
@@ -20,13 +20,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +43,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -51,11 +64,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>